<commit_message>
Penambahan Fitur & Sorting
+Fitur Search Excel
+Sorting Controller BODEksisting untuk Excel
</commit_message>
<xml_diff>
--- a/public/exp/BODAktualCimahi.xlsx
+++ b/public/exp/BODAktualCimahi.xlsx
@@ -9,13 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="20505" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel 29" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1646,18 +1658,18 @@
   <dimension ref="A1:AQ70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="9.140625" hidden="1" customWidth="1"/>
@@ -1861,7 +1873,7 @@
         <v>3.22</v>
       </c>
       <c r="M5" s="29">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="N5" s="29">
         <v>18</v>
@@ -1952,7 +1964,7 @@
       </c>
       <c r="AQ5" s="51">
         <f>(M5*AP5)*86.4</f>
-        <v>12.096000000000002</v>
+        <v>25.92</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
@@ -2645,7 +2657,7 @@
         <v>6.7</v>
       </c>
       <c r="M11" s="34">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N11" s="34">
         <v>28</v>
@@ -2736,7 +2748,7 @@
       </c>
       <c r="AQ11" s="51">
         <f t="shared" si="0"/>
-        <v>5310.1440000000002</v>
+        <v>7585.92</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
@@ -6877,7 +6889,7 @@
         <v>274.06079999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>5</v>
       </c>
@@ -7010,7 +7022,7 @@
         <v>412.12799999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>6</v>
       </c>
@@ -7278,7 +7290,7 @@
         <v>948.32640000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>8</v>
       </c>
@@ -7411,7 +7423,7 @@
         <v>2236.2912000000006</v>
       </c>
     </row>
-    <row r="59" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>9</v>
       </c>
@@ -8604,7 +8616,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">

</xml_diff>